<commit_message>
Borrow improvements and fixes.
</commit_message>
<xml_diff>
--- a/src/api-app/public/statement_report_template.xlsx
+++ b/src/api-app/public/statement_report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/CHACHI SDXC/Projects/Personal/SETEPID/saving_funds/src/api-app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F905F6F8-DE8B-E44A-9F66-29CFDA085147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8562A8F-BB65-E540-951B-984DAEBBB9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12540" yWindow="-26860" windowWidth="34860" windowHeight="23100" xr2:uid="{8BD8F66B-D635-0D49-A821-EBC64FBCC057}"/>
+    <workbookView xWindow="-12540" yWindow="-26880" windowWidth="34860" windowHeight="23100" activeTab="1" xr2:uid="{8BD8F66B-D635-0D49-A821-EBC64FBCC057}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATIVO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>ESTADO DE CUENTA</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>TOTAL APS.</t>
-  </si>
-  <si>
-    <t>TASA INT.</t>
-  </si>
-  <si>
-    <t>INTERESES</t>
   </si>
   <si>
     <t>RETIROS</t>
@@ -109,9 +103,6 @@
 EL RETIRO DE AHORRO MÁS RENDIMIENTOS, APLICA UNICAMENTE PARA AÑO CONCLUIDO.</t>
   </si>
   <si>
-    <t>REEMBOLSO</t>
-  </si>
-  <si>
     <t>NUEVO SALDO PARA EL {{CURRENT_YEAR}}:</t>
   </si>
   <si>
@@ -119,6 +110,12 @@
   </si>
   <si>
     <t>TOTAL EN FONDO DE AHORRO:</t>
+  </si>
+  <si>
+    <t>RENDIMIENTOS</t>
+  </si>
+  <si>
+    <t>TASA %</t>
   </si>
 </sst>
 </file>
@@ -176,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -206,50 +203,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -272,11 +225,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,20 +261,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,29 +276,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,124 +849,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2372613F-A5FF-FD4E-8B0F-5F949AB7F861}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="C15:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1015,10 +977,10 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1029,10 +991,10 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1043,259 +1005,253 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="E15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="I15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="21" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="21" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
@@ -1309,83 +1265,67 @@
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
+      <c r="B36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C41" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="C41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C1:J9"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="C37:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
+  <mergeCells count="26">
     <mergeCell ref="B21:J34"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="C10:J10"/>
@@ -1397,6 +1337,21 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="C1:J9"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="C37:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1408,124 +1363,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCB10D2-2852-5546-BA1D-B8F267879C8F}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1536,10 +1491,10 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1550,10 +1505,10 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1564,278 +1519,276 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="E15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="I15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="18"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="A21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
+      <c r="B24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
@@ -1849,62 +1802,78 @@
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="B37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C41" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="C41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="32">
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C1:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="H13:J13"/>
     <mergeCell ref="C38:I40"/>
     <mergeCell ref="C41:I41"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:J16"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H20:J20"/>
@@ -1917,23 +1886,6 @@
     <mergeCell ref="B37:J37"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
-    <mergeCell ref="C1:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>